<commit_message>
Initial commit: AR Automation V1
</commit_message>
<xml_diff>
--- a/Files/Cop.xlsx
+++ b/Files/Cop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AR Automation\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C085AFF-AEDB-454F-B81B-80E4271BFE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071DEE09-8383-4F4D-BE78-ACC1E60E232B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2C2130B2-D3AB-49E2-AC46-429D040882E3}"/>
   </bookViews>
@@ -540,7 +540,7 @@
   <dimension ref="A1:AJ345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>